<commit_message>
recycled code in outputs for report script. created a path in case the repository assets doesn't exist. Fixed fill between areas for big o chart.  split legend into two.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olya\Documents\Data Analytics\Semester 3\Computational Thinking with Algorithms\Sorting-Algorithms\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62111DAB-599D-4A36-ABAE-C86D342FFC10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,8 +28,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +92,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -152,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,27 +170,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,24 +204,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,19 +379,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="B1" s="1">
         <v>100</v>
       </c>
@@ -482,136 +427,136 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.7850000000000001</v>
+        <v>3.887</v>
       </c>
       <c r="C2">
-        <v>31.518999999999998</v>
+        <v>35.3</v>
       </c>
       <c r="D2">
-        <v>131.947</v>
+        <v>118.405</v>
       </c>
       <c r="E2">
-        <v>274.964</v>
+        <v>256.676</v>
       </c>
       <c r="F2">
-        <v>497.43200000000002</v>
+        <v>530.1849999999999</v>
       </c>
       <c r="G2">
-        <v>815.85199999999998</v>
+        <v>791.255</v>
       </c>
       <c r="H2">
-        <v>3014.6239999999998</v>
+        <v>3349.476</v>
       </c>
       <c r="I2">
-        <v>6892.9549999999999</v>
+        <v>6866.516</v>
       </c>
       <c r="J2">
-        <v>12195.24</v>
+        <v>11918.365</v>
       </c>
       <c r="K2">
-        <v>19098.915000000001</v>
+        <v>18299.652</v>
       </c>
       <c r="L2">
-        <v>26857.030999999999</v>
+        <v>26742.385</v>
       </c>
       <c r="M2">
-        <v>35472.593999999997</v>
+        <v>35897.407</v>
       </c>
       <c r="N2">
-        <v>50126.731</v>
+        <v>48638.799</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.4470000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="C3">
-        <v>5.0590000000000002</v>
+        <v>3.491</v>
       </c>
       <c r="D3">
-        <v>9.57</v>
+        <v>7.187</v>
       </c>
       <c r="E3">
-        <v>13.574999999999999</v>
+        <v>10.965</v>
       </c>
       <c r="F3">
-        <v>16.731000000000002</v>
+        <v>14.962</v>
       </c>
       <c r="G3">
-        <v>20.399999999999999</v>
+        <v>21.052</v>
       </c>
       <c r="H3">
-        <v>47.728999999999999</v>
+        <v>41.845</v>
       </c>
       <c r="I3">
-        <v>76.397000000000006</v>
+        <v>61.537</v>
       </c>
       <c r="J3">
-        <v>103.3</v>
+        <v>79.682</v>
       </c>
       <c r="K3">
-        <v>131.58099999999999</v>
+        <v>114.689</v>
       </c>
       <c r="L3">
-        <v>146.03100000000001</v>
+        <v>123.069</v>
       </c>
       <c r="M3">
-        <v>179.06899999999999</v>
+        <v>145.967</v>
       </c>
       <c r="N3">
-        <v>205.68700000000001</v>
+        <v>171.44</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.7410000000000001</v>
+        <v>2.497</v>
       </c>
       <c r="C4">
-        <v>9.3290000000000006</v>
+        <v>8.875999999999999</v>
       </c>
       <c r="D4">
-        <v>24.443999999999999</v>
+        <v>20.245</v>
       </c>
       <c r="E4">
-        <v>37.451999999999998</v>
+        <v>37.396</v>
       </c>
       <c r="F4">
-        <v>56.485999999999997</v>
+        <v>58.55</v>
       </c>
       <c r="G4">
-        <v>71.703000000000003</v>
+        <v>63.83</v>
       </c>
       <c r="H4">
-        <v>156.703</v>
+        <v>144.878</v>
       </c>
       <c r="I4">
-        <v>243.078</v>
+        <v>218.415</v>
       </c>
       <c r="J4">
-        <v>338.07</v>
+        <v>297.171</v>
       </c>
       <c r="K4">
-        <v>446.68400000000003</v>
+        <v>383.933</v>
       </c>
       <c r="L4">
-        <v>524.53</v>
+        <v>519.607</v>
       </c>
       <c r="M4">
-        <v>649.54399999999998</v>
+        <v>624.441</v>
       </c>
       <c r="N4">
-        <v>728.72199999999998</v>
+        <v>680.198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added bucket sort  and run the benchmark. Added libraries used in the project to the readme file. Separated excel output to its own function.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Insertion Sort</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Heap Sort</t>
+  </si>
+  <si>
+    <t>Bucket Sort</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,43 +435,43 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.887</v>
+        <v>5.786</v>
       </c>
       <c r="C2">
-        <v>35.3</v>
+        <v>30.617</v>
       </c>
       <c r="D2">
-        <v>118.405</v>
+        <v>217.22</v>
       </c>
       <c r="E2">
-        <v>256.676</v>
+        <v>354.355</v>
       </c>
       <c r="F2">
-        <v>530.1849999999999</v>
+        <v>633.509</v>
       </c>
       <c r="G2">
-        <v>791.255</v>
+        <v>1346.322</v>
       </c>
       <c r="H2">
-        <v>3349.476</v>
+        <v>3779.554</v>
       </c>
       <c r="I2">
-        <v>6866.516</v>
+        <v>7372.967</v>
       </c>
       <c r="J2">
-        <v>11918.365</v>
+        <v>12467.447</v>
       </c>
       <c r="K2">
-        <v>18299.652</v>
+        <v>20065.63</v>
       </c>
       <c r="L2">
-        <v>26742.385</v>
+        <v>32661.491</v>
       </c>
       <c r="M2">
-        <v>35897.407</v>
+        <v>39882.894</v>
       </c>
       <c r="N2">
-        <v>48638.799</v>
+        <v>49989.067</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -476,43 +479,43 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.4</v>
+        <v>1.806</v>
       </c>
       <c r="C3">
-        <v>3.491</v>
+        <v>5.083</v>
       </c>
       <c r="D3">
-        <v>7.187</v>
+        <v>8.292999999999999</v>
       </c>
       <c r="E3">
-        <v>10.965</v>
+        <v>11.575</v>
       </c>
       <c r="F3">
-        <v>14.962</v>
+        <v>16.359</v>
       </c>
       <c r="G3">
-        <v>21.052</v>
+        <v>20.746</v>
       </c>
       <c r="H3">
-        <v>41.845</v>
+        <v>60.944</v>
       </c>
       <c r="I3">
-        <v>61.537</v>
+        <v>101.428</v>
       </c>
       <c r="J3">
-        <v>79.682</v>
+        <v>123.274</v>
       </c>
       <c r="K3">
-        <v>114.689</v>
+        <v>112.798</v>
       </c>
       <c r="L3">
-        <v>123.069</v>
+        <v>152.692</v>
       </c>
       <c r="M3">
-        <v>145.967</v>
+        <v>214.231</v>
       </c>
       <c r="N3">
-        <v>171.44</v>
+        <v>201.571</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -520,43 +523,87 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.497</v>
+        <v>2.992</v>
       </c>
       <c r="C4">
-        <v>8.875999999999999</v>
+        <v>9.173999999999999</v>
       </c>
       <c r="D4">
-        <v>20.245</v>
+        <v>23.024</v>
       </c>
       <c r="E4">
-        <v>37.396</v>
+        <v>41.39</v>
       </c>
       <c r="F4">
-        <v>58.55</v>
+        <v>46.282</v>
       </c>
       <c r="G4">
-        <v>63.83</v>
+        <v>61.786</v>
       </c>
       <c r="H4">
-        <v>144.878</v>
+        <v>141.713</v>
       </c>
       <c r="I4">
-        <v>218.415</v>
+        <v>227.455</v>
       </c>
       <c r="J4">
-        <v>297.171</v>
+        <v>312.97</v>
       </c>
       <c r="K4">
-        <v>383.933</v>
+        <v>422.363</v>
       </c>
       <c r="L4">
-        <v>519.607</v>
+        <v>476.292</v>
       </c>
       <c r="M4">
-        <v>624.441</v>
+        <v>643.455</v>
       </c>
       <c r="N4">
-        <v>680.198</v>
+        <v>805.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.793</v>
+      </c>
+      <c r="C5">
+        <v>4.588</v>
+      </c>
+      <c r="D5">
+        <v>9.973000000000001</v>
+      </c>
+      <c r="E5">
+        <v>14.861</v>
+      </c>
+      <c r="F5">
+        <v>19.25</v>
+      </c>
+      <c r="G5">
+        <v>37.094</v>
+      </c>
+      <c r="H5">
+        <v>93.54900000000001</v>
+      </c>
+      <c r="I5">
+        <v>174.832</v>
+      </c>
+      <c r="J5">
+        <v>273.829</v>
+      </c>
+      <c r="K5">
+        <v>402.041</v>
+      </c>
+      <c r="L5">
+        <v>648.973</v>
+      </c>
+      <c r="M5">
+        <v>1074.378</v>
+      </c>
+      <c r="N5">
+        <v>980.1369999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added introsort into algorithms. Plots need adjustments
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Insertion Sort</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Bucket Sort</t>
+  </si>
+  <si>
+    <t>IntroSort</t>
   </si>
 </sst>
 </file>
@@ -383,13 +386,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
         <v>100</v>
       </c>
@@ -402,208 +405,90 @@
       <c r="E1" s="1">
         <v>750</v>
       </c>
-      <c r="F1" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G1" s="1">
-        <v>1250</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2500</v>
-      </c>
-      <c r="I1" s="1">
-        <v>3750</v>
-      </c>
-      <c r="J1" s="1">
-        <v>5000</v>
-      </c>
-      <c r="K1" s="1">
-        <v>6250</v>
-      </c>
-      <c r="L1" s="1">
-        <v>7500</v>
-      </c>
-      <c r="M1" s="1">
-        <v>8750</v>
-      </c>
-      <c r="N1" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.786</v>
+        <v>5.785</v>
       </c>
       <c r="C2">
-        <v>30.617</v>
+        <v>40.942</v>
       </c>
       <c r="D2">
-        <v>217.22</v>
+        <v>131.182</v>
       </c>
       <c r="E2">
-        <v>354.355</v>
-      </c>
-      <c r="F2">
-        <v>633.509</v>
-      </c>
-      <c r="G2">
-        <v>1346.322</v>
-      </c>
-      <c r="H2">
-        <v>3779.554</v>
-      </c>
-      <c r="I2">
-        <v>7372.967</v>
-      </c>
-      <c r="J2">
-        <v>12467.447</v>
-      </c>
-      <c r="K2">
-        <v>20065.63</v>
-      </c>
-      <c r="L2">
-        <v>32661.491</v>
-      </c>
-      <c r="M2">
-        <v>39882.894</v>
-      </c>
-      <c r="N2">
-        <v>49989.067</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>306.845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.806</v>
+        <v>1.208</v>
       </c>
       <c r="C3">
-        <v>5.083</v>
+        <v>3.815</v>
       </c>
       <c r="D3">
-        <v>8.292999999999999</v>
+        <v>8.086</v>
       </c>
       <c r="E3">
-        <v>11.575</v>
-      </c>
-      <c r="F3">
-        <v>16.359</v>
-      </c>
-      <c r="G3">
-        <v>20.746</v>
-      </c>
-      <c r="H3">
-        <v>60.944</v>
-      </c>
-      <c r="I3">
-        <v>101.428</v>
-      </c>
-      <c r="J3">
-        <v>123.274</v>
-      </c>
-      <c r="K3">
-        <v>112.798</v>
-      </c>
-      <c r="L3">
-        <v>152.692</v>
-      </c>
-      <c r="M3">
-        <v>214.231</v>
-      </c>
-      <c r="N3">
-        <v>201.571</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>11.974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.992</v>
+        <v>2.8</v>
       </c>
       <c r="C4">
-        <v>9.173999999999999</v>
+        <v>9.329000000000001</v>
       </c>
       <c r="D4">
-        <v>23.024</v>
+        <v>20.575</v>
       </c>
       <c r="E4">
-        <v>41.39</v>
-      </c>
-      <c r="F4">
-        <v>46.282</v>
-      </c>
-      <c r="G4">
-        <v>61.786</v>
-      </c>
-      <c r="H4">
-        <v>141.713</v>
-      </c>
-      <c r="I4">
-        <v>227.455</v>
-      </c>
-      <c r="J4">
-        <v>312.97</v>
-      </c>
-      <c r="K4">
-        <v>422.363</v>
-      </c>
-      <c r="L4">
-        <v>476.292</v>
-      </c>
-      <c r="M4">
-        <v>643.455</v>
-      </c>
-      <c r="N4">
-        <v>805.74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>33.546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.793</v>
+        <v>1.203</v>
       </c>
       <c r="C5">
-        <v>4.588</v>
+        <v>4.016</v>
       </c>
       <c r="D5">
-        <v>9.973000000000001</v>
+        <v>9.923</v>
       </c>
       <c r="E5">
-        <v>14.861</v>
-      </c>
-      <c r="F5">
-        <v>19.25</v>
-      </c>
-      <c r="G5">
-        <v>37.094</v>
-      </c>
-      <c r="H5">
-        <v>93.54900000000001</v>
-      </c>
-      <c r="I5">
-        <v>174.832</v>
-      </c>
-      <c r="J5">
-        <v>273.829</v>
-      </c>
-      <c r="K5">
-        <v>402.041</v>
-      </c>
-      <c r="L5">
-        <v>648.973</v>
-      </c>
-      <c r="M5">
-        <v>1074.378</v>
-      </c>
-      <c r="N5">
-        <v>980.1369999999999</v>
+        <v>14.175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.018</v>
+      </c>
+      <c r="C6">
+        <v>4.445</v>
+      </c>
+      <c r="D6">
+        <v>9.755000000000001</v>
+      </c>
+      <c r="E6">
+        <v>15.748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranged heap sort into nested function. Renamed the algorithms
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -411,16 +411,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.785</v>
+        <v>7.68</v>
       </c>
       <c r="C2">
-        <v>40.942</v>
+        <v>37.499</v>
       </c>
       <c r="D2">
-        <v>131.182</v>
+        <v>143.516</v>
       </c>
       <c r="E2">
-        <v>306.845</v>
+        <v>296.307</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,16 +428,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.208</v>
+        <v>1.496</v>
       </c>
       <c r="C3">
-        <v>3.815</v>
+        <v>3.69</v>
       </c>
       <c r="D3">
-        <v>8.086</v>
+        <v>8.577999999999999</v>
       </c>
       <c r="E3">
-        <v>11.974</v>
+        <v>16.354</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,16 +445,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.8</v>
+        <v>3.69</v>
       </c>
       <c r="C4">
-        <v>9.329000000000001</v>
+        <v>8.582000000000001</v>
       </c>
       <c r="D4">
-        <v>20.575</v>
+        <v>22.934</v>
       </c>
       <c r="E4">
-        <v>33.546</v>
+        <v>39.594</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -462,16 +462,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.203</v>
+        <v>1.6</v>
       </c>
       <c r="C5">
-        <v>4.016</v>
+        <v>4.973</v>
       </c>
       <c r="D5">
-        <v>9.923</v>
+        <v>10.276</v>
       </c>
       <c r="E5">
-        <v>14.175</v>
+        <v>16.551</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -479,16 +479,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.018</v>
+        <v>1.695</v>
       </c>
       <c r="C6">
-        <v>4.445</v>
+        <v>3.586</v>
       </c>
       <c r="D6">
-        <v>9.755000000000001</v>
+        <v>8.377000000000001</v>
       </c>
       <c r="E6">
-        <v>15.748</v>
+        <v>15.259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created another chart for big o (excluding insertion sort) otherwise the lines are too close to each other. Added dpcstring to bucket, quick and inserion sorts
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -411,16 +411,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7.68</v>
+        <v>5.485</v>
       </c>
       <c r="C2">
-        <v>37.499</v>
+        <v>33.414</v>
       </c>
       <c r="D2">
-        <v>143.516</v>
+        <v>132.642</v>
       </c>
       <c r="E2">
-        <v>296.307</v>
+        <v>304.588</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,16 +428,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.496</v>
+        <v>1.497</v>
       </c>
       <c r="C3">
-        <v>3.69</v>
+        <v>3.887</v>
       </c>
       <c r="D3">
-        <v>8.577999999999999</v>
+        <v>8.185</v>
       </c>
       <c r="E3">
-        <v>16.354</v>
+        <v>12.363</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,16 +445,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.69</v>
+        <v>3.59</v>
       </c>
       <c r="C4">
-        <v>8.582000000000001</v>
+        <v>10.173</v>
       </c>
       <c r="D4">
-        <v>22.934</v>
+        <v>24.33</v>
       </c>
       <c r="E4">
-        <v>39.594</v>
+        <v>39.997</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -462,16 +462,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.6</v>
+        <v>1.696</v>
       </c>
       <c r="C5">
-        <v>4.973</v>
+        <v>4.882</v>
       </c>
       <c r="D5">
-        <v>10.276</v>
+        <v>11.17</v>
       </c>
       <c r="E5">
-        <v>16.551</v>
+        <v>15.358</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -479,16 +479,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.695</v>
+        <v>1.396</v>
       </c>
       <c r="C6">
-        <v>3.586</v>
+        <v>3.989</v>
       </c>
       <c r="D6">
-        <v>8.377000000000001</v>
+        <v>10.472</v>
       </c>
       <c r="E6">
-        <v>15.259</v>
+        <v>19.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started writing a report. Rearranged assets script to have 4 plots since the lines merge - needed to zoom in.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olya\Documents\Data Analytics\Semester 3\Computational Thinking with Algorithms\Sorting-Algorithms\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3708BC-3B64-4E56-915C-9EF375A8A0BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Insertion Sort</t>
   </si>
@@ -29,13 +46,55 @@
   </si>
   <si>
     <t>IntroSort</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1250</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>3750</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>6250</t>
+  </si>
+  <si>
+    <t>7500</t>
+  </si>
+  <si>
+    <t>8750</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Sizes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,18 +146,132 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A64762B1-6628-4852-8A04-7D355A1C653A}" name="Table1" displayName="Table1" ref="A1:N6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:N6" xr:uid="{673A3D3F-FBDD-48BB-ACCD-212121136609}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{462E34AA-6C46-4DCA-8A77-1F7A45CDD9B2}" name="Sizes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{C81B6272-B0DB-4A50-AC6F-34FBF0BD2DE2}" name="100"/>
+    <tableColumn id="3" xr3:uid="{B03B0391-613B-43B7-9958-F16C4A3F6560}" name="250"/>
+    <tableColumn id="4" xr3:uid="{B71B0B9D-3BFE-4424-AD2B-879990BBB683}" name="500"/>
+    <tableColumn id="5" xr3:uid="{0C915DE5-3D81-4B5B-9E32-7BF3B6E06316}" name="750"/>
+    <tableColumn id="6" xr3:uid="{BD52F93F-660C-47F0-8A70-B4FEC969237E}" name="1000"/>
+    <tableColumn id="7" xr3:uid="{3AB3E82F-AC12-43CF-A5F0-49D884220EDF}" name="1250"/>
+    <tableColumn id="8" xr3:uid="{4C7C0ECA-F0AF-4089-AC17-42D36F91F182}" name="2500"/>
+    <tableColumn id="9" xr3:uid="{AAFBF606-21BF-4E41-B7C4-56B6EB9C729F}" name="3750"/>
+    <tableColumn id="10" xr3:uid="{26445711-09B9-4627-91FF-704C2E1F796C}" name="5000"/>
+    <tableColumn id="11" xr3:uid="{DACE2338-6DC8-4727-829E-F1552F14D211}" name="6250"/>
+    <tableColumn id="12" xr3:uid="{20A236AF-7344-4912-ABE8-60A2DACE5225}" name="7500"/>
+    <tableColumn id="13" xr3:uid="{C7E7D535-0005-4F4B-A785-939C388BA5D1}" name="8750"/>
+    <tableColumn id="14" xr3:uid="{17E15F05-F5D1-4C37-AFB7-9FCA9155107F}" name="10000"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,7 +317,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +349,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +401,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,113 +594,297 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="11" width="9.77734375" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1">
-        <v>100</v>
-      </c>
-      <c r="C1" s="1">
-        <v>250</v>
-      </c>
-      <c r="D1" s="1">
-        <v>500</v>
-      </c>
-      <c r="E1" s="1">
-        <v>750</v>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.485</v>
+        <v>8.6150000000000002</v>
       </c>
       <c r="C2">
-        <v>33.414</v>
+        <v>44.186999999999998</v>
       </c>
       <c r="D2">
-        <v>132.642</v>
+        <v>145.09399999999999</v>
       </c>
       <c r="E2">
-        <v>304.588</v>
+        <v>330.76</v>
+      </c>
+      <c r="F2">
+        <v>584.56899999999996</v>
+      </c>
+      <c r="G2">
+        <v>1038.7180000000001</v>
+      </c>
+      <c r="H2">
+        <v>3940.9580000000001</v>
+      </c>
+      <c r="I2">
+        <v>8683.3070000000007</v>
+      </c>
+      <c r="J2">
+        <v>16853.673999999999</v>
+      </c>
+      <c r="K2">
+        <v>26118.585999999999</v>
+      </c>
+      <c r="L2">
+        <v>36798.18</v>
+      </c>
+      <c r="M2">
+        <v>51102.482000000004</v>
+      </c>
+      <c r="N2">
+        <v>68049.178</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.497</v>
+        <v>2.1320000000000001</v>
       </c>
       <c r="C3">
-        <v>3.887</v>
+        <v>3.9940000000000002</v>
       </c>
       <c r="D3">
-        <v>8.185</v>
+        <v>8.7880000000000003</v>
       </c>
       <c r="E3">
-        <v>12.363</v>
+        <v>14.288</v>
+      </c>
+      <c r="F3">
+        <v>18.977</v>
+      </c>
+      <c r="G3">
+        <v>23.661000000000001</v>
+      </c>
+      <c r="H3">
+        <v>52.62</v>
+      </c>
+      <c r="I3">
+        <v>91.081999999999994</v>
+      </c>
+      <c r="J3">
+        <v>131.53100000000001</v>
+      </c>
+      <c r="K3">
+        <v>148.98699999999999</v>
+      </c>
+      <c r="L3">
+        <v>185.52600000000001</v>
+      </c>
+      <c r="M3">
+        <v>240.11699999999999</v>
+      </c>
+      <c r="N3">
+        <v>270.27300000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.59</v>
+        <v>3.9380000000000002</v>
       </c>
       <c r="C4">
-        <v>10.173</v>
+        <v>14.023999999999999</v>
       </c>
       <c r="D4">
-        <v>24.33</v>
+        <v>29.678000000000001</v>
       </c>
       <c r="E4">
-        <v>39.997</v>
+        <v>49.134999999999998</v>
+      </c>
+      <c r="F4">
+        <v>71.094999999999999</v>
+      </c>
+      <c r="G4">
+        <v>83.326999999999998</v>
+      </c>
+      <c r="H4">
+        <v>174.13</v>
+      </c>
+      <c r="I4">
+        <v>309.03500000000003</v>
+      </c>
+      <c r="J4">
+        <v>428.62400000000002</v>
+      </c>
+      <c r="K4">
+        <v>495.51400000000001</v>
+      </c>
+      <c r="L4">
+        <v>612.13900000000001</v>
+      </c>
+      <c r="M4">
+        <v>708.83199999999999</v>
+      </c>
+      <c r="N4">
+        <v>836.24800000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.696</v>
+        <v>1.5980000000000001</v>
       </c>
       <c r="C5">
-        <v>4.882</v>
+        <v>4.1790000000000003</v>
       </c>
       <c r="D5">
-        <v>11.17</v>
+        <v>10.327999999999999</v>
       </c>
       <c r="E5">
-        <v>15.358</v>
+        <v>16.611000000000001</v>
+      </c>
+      <c r="F5">
+        <v>22.959</v>
+      </c>
+      <c r="G5">
+        <v>47.140999999999998</v>
+      </c>
+      <c r="H5">
+        <v>76.722999999999999</v>
+      </c>
+      <c r="I5">
+        <v>150.642</v>
+      </c>
+      <c r="J5">
+        <v>242.875</v>
+      </c>
+      <c r="K5">
+        <v>371.101</v>
+      </c>
+      <c r="L5">
+        <v>519.63400000000001</v>
+      </c>
+      <c r="M5">
+        <v>703.35699999999997</v>
+      </c>
+      <c r="N5">
+        <v>1007.795</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.396</v>
+        <v>1.6739999999999999</v>
       </c>
       <c r="C6">
-        <v>3.989</v>
+        <v>5.0430000000000001</v>
       </c>
       <c r="D6">
-        <v>10.472</v>
+        <v>11.098000000000001</v>
       </c>
       <c r="E6">
-        <v>19.3</v>
+        <v>20.134</v>
+      </c>
+      <c r="F6">
+        <v>23.068000000000001</v>
+      </c>
+      <c r="G6">
+        <v>33.363999999999997</v>
+      </c>
+      <c r="H6">
+        <v>67.834999999999994</v>
+      </c>
+      <c r="I6">
+        <v>103.779</v>
+      </c>
+      <c r="J6">
+        <v>136.952</v>
+      </c>
+      <c r="K6">
+        <v>166.59200000000001</v>
+      </c>
+      <c r="L6">
+        <v>203.66200000000001</v>
+      </c>
+      <c r="M6">
+        <v>233.68899999999999</v>
+      </c>
+      <c r="N6">
+        <v>279.06700000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated report: added a diagram for insertion sort, extended introduction and benchmarking. Added assets into the resport as well.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olya\Documents\Data Analytics\Semester 3\Computational Thinking with Algorithms\Sorting-Algorithms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3708BC-3B64-4E56-915C-9EF375A8A0BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF62A709-46DE-4FBC-BBE8-CEB5EC5C025F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -270,7 +270,7 @@
     <tableColumn id="13" xr3:uid="{C7E7D535-0005-4F4B-A785-939C388BA5D1}" name="8750"/>
     <tableColumn id="14" xr3:uid="{17E15F05-F5D1-4C37-AFB7-9FCA9155107F}" name="10000"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -598,7 +598,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed array input sizes up to 15000, added description to bucket sort, started for introsort. Amended bucket and introsort diagrams. Simplified bucket sort algorithm.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -1,37 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olya\Documents\Data Analytics\Semester 3\Computational Thinking with Algorithms\Sorting-Algorithms\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF62A709-46DE-4FBC-BBE8-CEB5EC5C025F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Insertion Sort</t>
   </si>
@@ -45,56 +28,14 @@
     <t>Bucket Sort</t>
   </si>
   <si>
-    <t>IntroSort</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>750</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>1250</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>3750</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>6250</t>
-  </si>
-  <si>
-    <t>7500</t>
-  </si>
-  <si>
-    <t>8750</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>Sizes</t>
+    <t>Introsort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,132 +87,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A64762B1-6628-4852-8A04-7D355A1C653A}" name="Table1" displayName="Table1" ref="A1:N6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:N6" xr:uid="{673A3D3F-FBDD-48BB-ACCD-212121136609}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{462E34AA-6C46-4DCA-8A77-1F7A45CDD9B2}" name="Sizes" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{C81B6272-B0DB-4A50-AC6F-34FBF0BD2DE2}" name="100"/>
-    <tableColumn id="3" xr3:uid="{B03B0391-613B-43B7-9958-F16C4A3F6560}" name="250"/>
-    <tableColumn id="4" xr3:uid="{B71B0B9D-3BFE-4424-AD2B-879990BBB683}" name="500"/>
-    <tableColumn id="5" xr3:uid="{0C915DE5-3D81-4B5B-9E32-7BF3B6E06316}" name="750"/>
-    <tableColumn id="6" xr3:uid="{BD52F93F-660C-47F0-8A70-B4FEC969237E}" name="1000"/>
-    <tableColumn id="7" xr3:uid="{3AB3E82F-AC12-43CF-A5F0-49D884220EDF}" name="1250"/>
-    <tableColumn id="8" xr3:uid="{4C7C0ECA-F0AF-4089-AC17-42D36F91F182}" name="2500"/>
-    <tableColumn id="9" xr3:uid="{AAFBF606-21BF-4E41-B7C4-56B6EB9C729F}" name="3750"/>
-    <tableColumn id="10" xr3:uid="{26445711-09B9-4627-91FF-704C2E1F796C}" name="5000"/>
-    <tableColumn id="11" xr3:uid="{DACE2338-6DC8-4727-829E-F1552F14D211}" name="6250"/>
-    <tableColumn id="12" xr3:uid="{20A236AF-7344-4912-ABE8-60A2DACE5225}" name="7500"/>
-    <tableColumn id="13" xr3:uid="{C7E7D535-0005-4F4B-A785-939C388BA5D1}" name="8750"/>
-    <tableColumn id="14" xr3:uid="{17E15F05-F5D1-4C37-AFB7-9FCA9155107F}" name="10000"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -317,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,27 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,24 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,297 +385,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="11" width="9.77734375" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
+    <row r="1" spans="1:14">
+      <c r="B1" s="1">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1">
+        <v>250</v>
+      </c>
+      <c r="D1" s="1">
+        <v>500</v>
+      </c>
+      <c r="E1" s="1">
+        <v>750</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1250</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2500</v>
+      </c>
+      <c r="I1" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J1" s="1">
+        <v>6250</v>
+      </c>
+      <c r="K1" s="1">
+        <v>7500</v>
+      </c>
+      <c r="L1" s="1">
+        <v>8750</v>
+      </c>
+      <c r="M1" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N1" s="1">
+        <v>15000</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8.6150000000000002</v>
+        <v>4.388</v>
       </c>
       <c r="C2">
-        <v>44.186999999999998</v>
+        <v>29.921</v>
       </c>
       <c r="D2">
-        <v>145.09399999999999</v>
+        <v>130.352</v>
       </c>
       <c r="E2">
-        <v>330.76</v>
+        <v>264.691</v>
       </c>
       <c r="F2">
-        <v>584.56899999999996</v>
+        <v>510.336</v>
       </c>
       <c r="G2">
-        <v>1038.7180000000001</v>
+        <v>821.299</v>
       </c>
       <c r="H2">
-        <v>3940.9580000000001</v>
+        <v>3111.087</v>
       </c>
       <c r="I2">
-        <v>8683.3070000000007</v>
+        <v>12351.283</v>
       </c>
       <c r="J2">
-        <v>16853.673999999999</v>
+        <v>20688.085</v>
       </c>
       <c r="K2">
-        <v>26118.585999999999</v>
+        <v>29430.363</v>
       </c>
       <c r="L2">
-        <v>36798.18</v>
+        <v>41193.344</v>
       </c>
       <c r="M2">
-        <v>51102.482000000004</v>
+        <v>52562.576</v>
       </c>
       <c r="N2">
-        <v>68049.178</v>
+        <v>124356.048</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.1320000000000001</v>
+        <v>1.665</v>
       </c>
       <c r="C3">
-        <v>3.9940000000000002</v>
+        <v>4.722</v>
       </c>
       <c r="D3">
-        <v>8.7880000000000003</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="E3">
-        <v>14.288</v>
+        <v>13.919</v>
       </c>
       <c r="F3">
-        <v>18.977</v>
+        <v>18.588</v>
       </c>
       <c r="G3">
-        <v>23.661000000000001</v>
+        <v>24.922</v>
       </c>
       <c r="H3">
-        <v>52.62</v>
+        <v>52.308</v>
       </c>
       <c r="I3">
-        <v>91.081999999999994</v>
+        <v>112.571</v>
       </c>
       <c r="J3">
-        <v>131.53100000000001</v>
+        <v>135.208</v>
       </c>
       <c r="K3">
-        <v>148.98699999999999</v>
+        <v>160.1</v>
       </c>
       <c r="L3">
-        <v>185.52600000000001</v>
+        <v>194.436</v>
       </c>
       <c r="M3">
-        <v>240.11699999999999</v>
+        <v>228.16</v>
       </c>
       <c r="N3">
-        <v>270.27300000000002</v>
+        <v>354.638</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.9380000000000002</v>
+        <v>3.004</v>
       </c>
       <c r="C4">
-        <v>14.023999999999999</v>
+        <v>10.069</v>
       </c>
       <c r="D4">
-        <v>29.678000000000001</v>
+        <v>22.19</v>
       </c>
       <c r="E4">
-        <v>49.134999999999998</v>
+        <v>36.54</v>
       </c>
       <c r="F4">
-        <v>71.094999999999999</v>
+        <v>53.57</v>
       </c>
       <c r="G4">
-        <v>83.326999999999998</v>
+        <v>66.79900000000001</v>
       </c>
       <c r="H4">
-        <v>174.13</v>
+        <v>149.022</v>
       </c>
       <c r="I4">
-        <v>309.03500000000003</v>
+        <v>334.647</v>
       </c>
       <c r="J4">
-        <v>428.62400000000002</v>
+        <v>426.173</v>
       </c>
       <c r="K4">
-        <v>495.51400000000001</v>
+        <v>513.455</v>
       </c>
       <c r="L4">
-        <v>612.13900000000001</v>
+        <v>621.443</v>
       </c>
       <c r="M4">
-        <v>708.83199999999999</v>
+        <v>696.033</v>
       </c>
       <c r="N4">
-        <v>836.24800000000005</v>
+        <v>1111.549</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.5980000000000001</v>
+        <v>0.304</v>
       </c>
       <c r="C5">
-        <v>4.1790000000000003</v>
+        <v>0.931</v>
       </c>
       <c r="D5">
-        <v>10.327999999999999</v>
+        <v>2.574</v>
       </c>
       <c r="E5">
-        <v>16.611000000000001</v>
+        <v>4.478</v>
       </c>
       <c r="F5">
-        <v>22.959</v>
+        <v>7.141</v>
       </c>
       <c r="G5">
-        <v>47.140999999999998</v>
+        <v>22.164</v>
       </c>
       <c r="H5">
-        <v>76.722999999999999</v>
+        <v>40.045</v>
       </c>
       <c r="I5">
-        <v>150.642</v>
+        <v>171.452</v>
       </c>
       <c r="J5">
-        <v>242.875</v>
+        <v>280.187</v>
       </c>
       <c r="K5">
-        <v>371.101</v>
+        <v>415.914</v>
       </c>
       <c r="L5">
-        <v>519.63400000000001</v>
+        <v>591.241</v>
       </c>
       <c r="M5">
-        <v>703.35699999999997</v>
+        <v>769.375</v>
       </c>
       <c r="N5">
-        <v>1007.795</v>
+        <v>1830.523</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.6739999999999999</v>
+        <v>1.294</v>
       </c>
       <c r="C6">
-        <v>5.0430000000000001</v>
+        <v>3.683</v>
       </c>
       <c r="D6">
-        <v>11.098000000000001</v>
+        <v>9.333</v>
       </c>
       <c r="E6">
-        <v>20.134</v>
+        <v>12.746</v>
       </c>
       <c r="F6">
-        <v>23.068000000000001</v>
+        <v>16.716</v>
       </c>
       <c r="G6">
-        <v>33.363999999999997</v>
+        <v>24.04</v>
       </c>
       <c r="H6">
-        <v>67.834999999999994</v>
+        <v>50.665</v>
       </c>
       <c r="I6">
-        <v>103.779</v>
+        <v>110.009</v>
       </c>
       <c r="J6">
-        <v>136.952</v>
+        <v>143.098</v>
       </c>
       <c r="K6">
-        <v>166.59200000000001</v>
+        <v>171.766</v>
       </c>
       <c r="L6">
-        <v>203.66200000000001</v>
+        <v>202.074</v>
       </c>
       <c r="M6">
-        <v>233.68899999999999</v>
+        <v>244.528</v>
       </c>
       <c r="N6">
-        <v>279.06700000000001</v>
+        <v>362.709</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced numpy with random package and shortened the benchmark runner function. . finished the report.
</commit_message>
<xml_diff>
--- a/assets/benchmark_results.xlsx
+++ b/assets/benchmark_results.xlsx
@@ -438,43 +438,43 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.124</v>
+        <v>3.041</v>
       </c>
       <c r="C2">
-        <v>14.059</v>
+        <v>21.59</v>
       </c>
       <c r="D2">
-        <v>59.62</v>
+        <v>90.587</v>
       </c>
       <c r="E2">
-        <v>143.972</v>
+        <v>241.919</v>
       </c>
       <c r="F2">
-        <v>258.343</v>
+        <v>459.373</v>
       </c>
       <c r="G2">
-        <v>408.654</v>
+        <v>804.925</v>
       </c>
       <c r="H2">
-        <v>1675.633</v>
+        <v>2106.572</v>
       </c>
       <c r="I2">
-        <v>6732.687</v>
+        <v>8517.050999999999</v>
       </c>
       <c r="J2">
-        <v>10446.705</v>
+        <v>12356.957</v>
       </c>
       <c r="K2">
-        <v>15062.647</v>
+        <v>18223.146</v>
       </c>
       <c r="L2">
-        <v>20508.873</v>
+        <v>28473.934</v>
       </c>
       <c r="M2">
-        <v>26850.861</v>
+        <v>33703.88</v>
       </c>
       <c r="N2">
-        <v>60559.383</v>
+        <v>73387.905</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -482,43 +482,43 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.542</v>
+        <v>1.222</v>
       </c>
       <c r="C3">
-        <v>4.687</v>
+        <v>2.74</v>
       </c>
       <c r="D3">
-        <v>6.248</v>
+        <v>3.974</v>
       </c>
       <c r="E3">
-        <v>12.606</v>
+        <v>7.828</v>
       </c>
       <c r="F3">
-        <v>15.621</v>
+        <v>10.384</v>
       </c>
       <c r="G3">
-        <v>20.432</v>
+        <v>12.641</v>
       </c>
       <c r="H3">
-        <v>39.163</v>
+        <v>37.459</v>
       </c>
       <c r="I3">
-        <v>86.16200000000001</v>
+        <v>73.06399999999999</v>
       </c>
       <c r="J3">
-        <v>107.899</v>
+        <v>84.658</v>
       </c>
       <c r="K3">
-        <v>134.592</v>
+        <v>127.222</v>
       </c>
       <c r="L3">
-        <v>150.197</v>
+        <v>140.433</v>
       </c>
       <c r="M3">
-        <v>185.032</v>
+        <v>169.978</v>
       </c>
       <c r="N3">
-        <v>273.373</v>
+        <v>241.43</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -526,43 +526,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.562</v>
+        <v>1.543</v>
       </c>
       <c r="C4">
-        <v>4.686</v>
+        <v>4.479</v>
       </c>
       <c r="D4">
-        <v>10.935</v>
+        <v>10.483</v>
       </c>
       <c r="E4">
-        <v>15.621</v>
+        <v>16.908</v>
       </c>
       <c r="F4">
-        <v>23.432</v>
+        <v>23.068</v>
       </c>
       <c r="G4">
-        <v>28.118</v>
+        <v>31.06</v>
       </c>
       <c r="H4">
-        <v>68.73399999999999</v>
+        <v>69.398</v>
       </c>
       <c r="I4">
-        <v>147.086</v>
+        <v>206.932</v>
       </c>
       <c r="J4">
-        <v>190.58</v>
+        <v>202.412</v>
       </c>
       <c r="K4">
-        <v>231.671</v>
+        <v>290.046</v>
       </c>
       <c r="L4">
-        <v>276.498</v>
+        <v>316.534</v>
       </c>
       <c r="M4">
-        <v>322.027</v>
+        <v>389.566</v>
       </c>
       <c r="N4">
-        <v>504.809</v>
+        <v>584.6</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -570,43 +570,43 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.209</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.412</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.518</v>
       </c>
       <c r="E5">
-        <v>1.562</v>
+        <v>0.539</v>
       </c>
       <c r="F5">
-        <v>1.562</v>
+        <v>0.873</v>
       </c>
       <c r="G5">
-        <v>4.687</v>
+        <v>6.104</v>
       </c>
       <c r="H5">
-        <v>4.686</v>
+        <v>3.231</v>
       </c>
       <c r="I5">
-        <v>4.686</v>
+        <v>8.733000000000001</v>
       </c>
       <c r="J5">
-        <v>12.497</v>
+        <v>12.706</v>
       </c>
       <c r="K5">
-        <v>14.059</v>
+        <v>14.062</v>
       </c>
       <c r="L5">
-        <v>17.184</v>
+        <v>19.19</v>
       </c>
       <c r="M5">
-        <v>15.621</v>
+        <v>21.531</v>
       </c>
       <c r="N5">
-        <v>26.556</v>
+        <v>27.872</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -614,43 +614,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.562</v>
+        <v>0.4</v>
       </c>
       <c r="C6">
-        <v>1.562</v>
+        <v>2.927</v>
       </c>
       <c r="D6">
-        <v>3.124</v>
+        <v>6.755</v>
       </c>
       <c r="E6">
-        <v>6.249</v>
+        <v>10.262</v>
       </c>
       <c r="F6">
-        <v>7.811</v>
+        <v>12.015</v>
       </c>
       <c r="G6">
-        <v>10.935</v>
+        <v>11.775</v>
       </c>
       <c r="H6">
-        <v>23.432</v>
+        <v>22.814</v>
       </c>
       <c r="I6">
-        <v>48.426</v>
+        <v>51.243</v>
       </c>
       <c r="J6">
-        <v>64.048</v>
+        <v>64.962</v>
       </c>
       <c r="K6">
-        <v>78.235</v>
+        <v>94.54900000000001</v>
       </c>
       <c r="L6">
-        <v>93.836</v>
+        <v>120.797</v>
       </c>
       <c r="M6">
-        <v>104.663</v>
+        <v>109.447</v>
       </c>
       <c r="N6">
-        <v>164.509</v>
+        <v>233.377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>